<commit_message>
Update RTOS componenents, start Etapa 2 slides
</commit_message>
<xml_diff>
--- a/docs/Especificacao do Software.xlsx
+++ b/docs/Especificacao do Software.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel.brunheira\Git\pessoal\project-reggae\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE02A919-F845-481C-8554-4F184C1EEF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A8798F-AC9D-487D-A339-627EC2AF3AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{954C87E8-33D2-4ED4-AA5D-1C935BF763B1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{954C87E8-33D2-4ED4-AA5D-1C935BF763B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tarefas" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>Gerenciar botões</t>
   </si>
@@ -183,6 +183,24 @@
   </si>
   <si>
     <t>day</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Tamanho</t>
+  </si>
+  <si>
+    <t>Dado</t>
+  </si>
+  <si>
+    <t>Tarefa</t>
+  </si>
+  <si>
+    <t>Prioridade</t>
   </si>
 </sst>
 </file>
@@ -224,13 +242,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,21 +587,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49ED95AB-ED45-423D-9B78-F82C89FC3E6F}">
-  <dimension ref="B2:E13"/>
+  <dimension ref="B2:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="67.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
@@ -591,7 +612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -604,8 +625,12 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -618,8 +643,11 @@
       <c r="E4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -629,48 +657,68 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
+      <c r="I13" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I11:J11"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -767,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267159DF-7819-4979-A1BC-F659E5716480}">
   <dimension ref="B3:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>